<commit_message>
Updated Meeting documents during our meeting
</commit_message>
<xml_diff>
--- a/Meeting Documents/Meeting Atendance.xlsx
+++ b/Meeting Documents/Meeting Atendance.xlsx
@@ -1,30 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr showInkAnnotation="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zach_\OneDrive\Second Year\group software\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravi_\Documents\GitHub\Treasure-Hunt\Meeting Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B667473B-A9EF-40B8-89F1-F596626C998A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12612"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -67,7 +58,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -429,11 +420,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,6 +492,19 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>43868</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.51736111111111105</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated time for last meeting
</commit_message>
<xml_diff>
--- a/Meeting Documents/Meeting Atendance.xlsx
+++ b/Meeting Documents/Meeting Atendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravi_\Documents\GitHub\Treasure-Hunt\Meeting Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B667473B-A9EF-40B8-89F1-F596626C998A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5E7905-546A-443C-9BD3-8552B64E1890}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>times</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>16:30 - 17:30</t>
+  </si>
+  <si>
+    <t>12:25 - 13:30</t>
   </si>
 </sst>
 </file>
@@ -424,7 +427,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -496,8 +499,8 @@
       <c r="A5" s="2">
         <v>43868</v>
       </c>
-      <c r="B5" s="3">
-        <v>0.51736111111111105</v>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>

</xml_diff>

<commit_message>
Updated Meeting Attendance document
</commit_message>
<xml_diff>
--- a/Meeting Documents/Meeting Atendance.xlsx
+++ b/Meeting Documents/Meeting Atendance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ravi_\Documents\GitHub\Treasure-Hunt\Meeting Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5E7905-546A-443C-9BD3-8552B64E1890}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E18C42-BF4C-4AD8-B5FA-B26C9753EB51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,35 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>times</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>dates</t>
   </si>
   <si>
-    <t>people</t>
-  </si>
-  <si>
-    <t>ravi</t>
-  </si>
-  <si>
-    <t>ben</t>
-  </si>
-  <si>
-    <t>zach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">harry </t>
-  </si>
-  <si>
-    <t>freddie</t>
-  </si>
-  <si>
-    <t>adam</t>
-  </si>
-  <si>
     <t>12:30-2:15</t>
   </si>
   <si>
@@ -56,6 +32,39 @@
   </si>
   <si>
     <t>12:25 - 13:30</t>
+  </si>
+  <si>
+    <t>Ravi</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>Zach</t>
+  </si>
+  <si>
+    <t>Harry</t>
+  </si>
+  <si>
+    <t>Freddie</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>15:00 - 16:10</t>
+  </si>
+  <si>
+    <t>Adam - family situation</t>
+  </si>
+  <si>
+    <t>Zach - assessment centre</t>
+  </si>
+  <si>
+    <t>Team Members</t>
+  </si>
+  <si>
+    <t>Times</t>
   </si>
 </sst>
 </file>
@@ -104,11 +113,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -424,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -436,43 +446,43 @@
     <col min="2" max="2" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>43861</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -481,12 +491,12 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>43864</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -495,18 +505,38 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>43868</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
+      <c r="J5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>43872</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="4"/>
+      <c r="J6" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>